<commit_message>
integration tests for named items
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/DataModelNamedItems_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/DataModelNamedItems_Test.xlsx
@@ -13,6 +13,7 @@
     <definedName name="Coef_One">12.9</definedName>
     <definedName name="My_Function">SUM(Sheet1!$A$2,Sheet1!$A$3)</definedName>
     <definedName name="My_Grades">Sheet1!$A$2:$A$5</definedName>
+    <definedName name="My_Values">Sheet1!$A$2,Sheet1!$A$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -382,7 +383,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,6 +430,10 @@
       <c r="A5">
         <v>9</v>
       </c>
+      <c r="C5">
+        <f>SUM(My_Values)</f>
+        <v>17.100000000000001</v>
+      </c>
       <c r="E5">
         <f>C2-C3-My_Function</f>
         <v>6.875</v>

</xml_diff>